<commit_message>
添加StudentServerInter接口public String getStudentPreTime(week, day time)
</commit_message>
<xml_diff>
--- a/FYP_System_Bug_Collection.xlsx
+++ b/FYP_System_Bug_Collection.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -52,40 +60,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>Teacher account</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-      </rPr>
-      <t>可以重复</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>coordinator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-      </rPr>
-      <t>加入一个新老师</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>account</t>
     </r>
     <r>
       <rPr>
@@ -175,12 +149,119 @@
     </r>
   </si>
   <si>
+    <t>teacher-editTopic</t>
+  </si>
+  <si>
+    <t>set opentime时间设置错误提示信息</t>
+  </si>
+  <si>
+    <t>建议</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>coordinator-set opentime</t>
+  </si>
+  <si>
+    <t>teacher index 提示信息</t>
+  </si>
+  <si>
+    <t>teacher-index</t>
+  </si>
+  <si>
+    <t>teacher logut</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>topiclist表格</t>
+  </si>
+  <si>
+    <t>teacher－topiclist</t>
+  </si>
+  <si>
+    <t>student-chooseTopic</t>
+  </si>
+  <si>
+    <t>groupmember info页面</t>
+  </si>
+  <si>
+    <t>student-groupmember info</t>
+  </si>
+  <si>
+    <t>严重</t>
+  </si>
+  <si>
+    <t>teacher-chooseObserver</t>
+  </si>
+  <si>
+    <t>teacher－chooseObserver</t>
+  </si>
+  <si>
+    <t>添加三个时间设置框</t>
+  </si>
+  <si>
+    <t>coordinator- set opentime</t>
+  </si>
+  <si>
+    <t>chooseExaminer</t>
+  </si>
+  <si>
+    <t>student-chooseExaminer</t>
+  </si>
+  <si>
+    <t>计算打印时间表时间</t>
+  </si>
+  <si>
+    <t>StudentServerInter</t>
+  </si>
+  <si>
+    <t>导航栏顺序</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
       </rPr>
+      <t>coordinator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>加入一个新老师</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>可以重复</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
       <t>uploadTopic</t>
     </r>
     <r>
@@ -189,168 +270,634 @@
         <color indexed="8"/>
         <rFont val="宋体"/>
       </rPr>
+      <t>输入可以为空</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>uploadTopic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
       <t>页面点击topiclist不能返回</t>
     </r>
-  </si>
-  <si>
-    <t>teacher-editTopic</t>
-  </si>
-  <si>
-    <t>set opentime时间设置错误提示信息</t>
-  </si>
-  <si>
-    <t>改成：Operation failed! Set xxx error! You can’t select the open time in the same date.</t>
-  </si>
-  <si>
-    <t>建议</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
-    <t>coordinator-set opentime</t>
-  </si>
-  <si>
-    <t>teacher index 提示信息</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>改成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Microsoft Tai Le"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Operation failed! Set xxx error! You can’t select the open time in the same date.</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>主页提示信息为空</t>
-  </si>
-  <si>
-    <t>teacher-index</t>
-  </si>
-  <si>
-    <t>teacher logut</t>
-  </si>
-  <si>
-    <t>用户名显示 logout提示</t>
-  </si>
-  <si>
-    <t>teacher</t>
-  </si>
-  <si>
-    <t>edittopic页面添加按钮</t>
-  </si>
-  <si>
-    <t>添加一个cancel button</t>
-  </si>
-  <si>
-    <t>edittopic下拉框</t>
-  </si>
-  <si>
-    <t>学分 individual 学生数量有搜索框</t>
-  </si>
-  <si>
-    <t>topiclist表格</t>
-  </si>
-  <si>
-    <t>group topic添加搜索 按钮放到同一行</t>
-  </si>
-  <si>
-    <t>teacher－topiclist</t>
-  </si>
-  <si>
-    <t>group topic supervisor无法显示多人</t>
-  </si>
-  <si>
-    <t>viewtopic时间段</t>
-  </si>
-  <si>
-    <t>没有viewtopic限制时间段</t>
-  </si>
-  <si>
-    <t>student-chooseTopic</t>
-  </si>
-  <si>
-    <t>drop topic没有确认提示框</t>
-  </si>
-  <si>
-    <t>已选topic编号</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>用户名显示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>提示</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>edittopic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>页面添加按钮</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>添加一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>cancel button</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>edittopic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>下拉框</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>学分</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> individual </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>学生数量有搜索框</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>group topic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>添加搜索</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>按钮放到同一行</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>topiclist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>表格</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>group topic supervisor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>无法显示多人</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>viewtopic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>时间段</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>没有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>viewtopic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>限制时间段</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>drop topic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>没有确认提示框</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>drop topic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>没有确认提示框</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>已选</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>topic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>编号</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>去掉编号显示</t>
-  </si>
-  <si>
-    <t>groupmember info页面</t>
-  </si>
-  <si>
-    <t>member下拉选框默认为please select</t>
-  </si>
-  <si>
-    <t>student-groupmember info</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>member</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>下拉选框默认为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>please select</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>chooseTopic</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>添加表格搜索功能</t>
-  </si>
-  <si>
-    <t>提交时检测成员是否选择其他项目 在groupmember info页面提示 cancel无功能</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>groupmember info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>页面</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>提交时检测成员是否选择其他项目</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>groupmember info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>页面提示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> cancel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>无功能</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>chooseObserver</t>
-  </si>
-  <si>
-    <t>没有选中的项目也能选observer</t>
-  </si>
-  <si>
-    <t>严重</t>
-  </si>
-  <si>
-    <t>teacher-chooseObserver</t>
-  </si>
-  <si>
-    <t>observer下拉选框为please select</t>
-  </si>
-  <si>
-    <t>teacher－chooseObserver</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>没有选中的项目也能选</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>observer</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>observer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Kaiti SC Black"/>
+      </rPr>
+      <t>下拉选框为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>please select</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>setOpentime</t>
-  </si>
-  <si>
-    <t>添加三个时间设置框</t>
-  </si>
-  <si>
-    <t>coordinator- set opentime</t>
-  </si>
-  <si>
-    <t>chooseExaminer</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>链接选老师无验证</t>
-  </si>
-  <si>
-    <t>student-chooseExaminer</t>
-  </si>
-  <si>
-    <t>选observer时没有验证是否是supervisor，s显示名字换成name不是id</t>
-  </si>
-  <si>
-    <t>计算打印时间表时间</t>
-  </si>
-  <si>
-    <t>添加StudentServerInter接口String getStudentPreTime(week, day time)</t>
-  </si>
-  <si>
-    <t>StudentServerInter</t>
-  </si>
-  <si>
-    <t>导航栏顺序</t>
-  </si>
-  <si>
-    <t>更改导航栏顺序 删clear project</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>选</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>observer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>时没有验证是否是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>supervisor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>显示名字换成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>不是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>添加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>StudentServerInter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>接口</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>String getStudentPreTime(week, day time)</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>更改导航栏顺序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+      </rPr>
+      <t>删</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>clear project</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -358,41 +905,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="11"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="宋体"/>
     </font>
@@ -425,6 +937,32 @@
       <sz val="10"/>
       <color indexed="11"/>
       <name val="宋体"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Kaiti SC Black"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Microsoft Tai Le"/>
     </font>
   </fonts>
   <fills count="5">
@@ -655,167 +1193,479 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="65">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="44">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="65">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffc0504d"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00b050"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff4f81bd"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffb8cce4"/>
-      <rgbColor rgb="ffdbe5f1"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFC0504D"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00B050"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFB8CCE4"/>
+      <rgbColor rgb="FFDBE5F1"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -829,7 +1679,7 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>161449</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Shape 2"/>
         <xdr:cNvSpPr/>
@@ -859,7 +1709,7 @@
           </a:cxnLst>
           <a:rect l="0" t="0" r="r" b="b"/>
           <a:pathLst>
-            <a:path w="21600" h="21600" fill="norm" stroke="1" extrusionOk="0">
+            <a:path w="21600" h="21600" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -907,8 +1757,10 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
-          <a:prstTxWarp prst="textNoShape"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle>
@@ -1005,7 +1857,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1029,7 +1881,7 @@
             </a:rPr>
             <a:t>文档参数说明：</a:t>
           </a:r>
-          <a:endParaRPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+          <a:endParaRPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -1074,7 +1926,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1099,7 +1951,7 @@
             <a:t>严重性：</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="C0504D"/>
               </a:solidFill>
@@ -1124,7 +1976,7 @@
             <a:t>崩溃（系统崩溃或数据丢失）</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1149,7 +2001,7 @@
             <a:t>，</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
@@ -1174,7 +2026,7 @@
             <a:t>严重（主要功能问题）</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1199,7 +2051,7 @@
             <a:t>，一般（次要功能问题），</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
@@ -1223,7 +2075,7 @@
             </a:rPr>
             <a:t>建议（细微问题或建议）</a:t>
           </a:r>
-          <a:endParaRPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+          <a:endParaRPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
             <a:solidFill>
               <a:srgbClr val="00B050"/>
             </a:solidFill>
@@ -1268,7 +2120,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1293,7 +2145,7 @@
             <a:t>优先级：</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1318,7 +2170,7 @@
             <a:t>p1: </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1343,7 +2195,7 @@
             <a:t>需要立即解决的问题</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1368,7 +2220,7 @@
             <a:t>(Now); p2: </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1393,7 +2245,7 @@
             <a:t>需要在指定时间内解决的问题</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1418,7 +2270,7 @@
             <a:t>(Need to be fixed in N days); p3: </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1443,7 +2295,7 @@
             <a:t>需要在指定时间内解决的问题</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1468,7 +2320,7 @@
             <a:t>(Need to be fixed in N days); p4: </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1493,7 +2345,7 @@
             <a:t>资源充沛时解决的问题</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1517,7 +2369,7 @@
             </a:rPr>
             <a:t>(Fix or not) </a:t>
           </a:r>
-          <a:endParaRPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+          <a:endParaRPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -1562,7 +2414,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1587,7 +2439,7 @@
             <a:t>解决：未解决，</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
@@ -1624,17 +2476,339 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K26"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+  <a:themeElements>
+    <a:clrScheme name="办公室">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="办公室">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="办公室">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="14" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.75" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.4531" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.2188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
@@ -1642,623 +2816,622 @@
     <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.75" style="1" customWidth="1"/>
-    <col min="12" max="256" width="7.75" style="1" customWidth="1"/>
+    <col min="11" max="256" width="7.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:11" ht="19" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="3">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="4">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="F2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s" s="9">
+      <c r="G2" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s" s="10">
-        <v>15</v>
       </c>
       <c r="H2" s="11">
         <v>41942</v>
       </c>
-      <c r="I2" t="s" s="7">
+      <c r="I2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="12">
-        <v>17</v>
-      </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" ht="19" customHeight="1">
+    <row r="3" spans="1:11" ht="19" customHeight="1">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="14">
+      <c r="B3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s" s="14">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="15">
+      <c r="E3" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s" s="16">
-        <v>20</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="18">
         <v>41990</v>
       </c>
-      <c r="I3" t="s" s="14">
-        <v>21</v>
+      <c r="I3" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" ht="19" customHeight="1">
+    <row r="4" spans="1:11" ht="19" customHeight="1">
       <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s" s="22">
+      <c r="B4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s" s="21">
-        <v>13</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
       <c r="H4" s="24">
         <v>41990</v>
       </c>
-      <c r="I4" t="s" s="21">
-        <v>24</v>
+      <c r="I4" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" ht="18" customHeight="1">
+    <row r="5" spans="1:11" ht="18" customHeight="1">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="14">
+      <c r="B5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s" s="14">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="26">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="16">
-        <v>28</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="18">
         <v>41991</v>
       </c>
-      <c r="I5" t="s" s="14">
-        <v>29</v>
+      <c r="I5" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" ht="18" customHeight="1">
+    <row r="6" spans="1:11" ht="18" customHeight="1">
       <c r="A6" s="20">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="21">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s" s="21">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s" s="22">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s" s="21">
-        <v>13</v>
+      <c r="B6" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
       <c r="H6" s="24">
         <v>41990</v>
       </c>
-      <c r="I6" t="s" s="21">
-        <v>32</v>
+      <c r="I6" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" ht="18" customHeight="1">
+    <row r="7" spans="1:11" ht="18" customHeight="1">
       <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="14">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s" s="14">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s" s="15">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s" s="16">
-        <v>13</v>
+      <c r="B7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="18">
         <v>41990</v>
       </c>
-      <c r="I7" t="s" s="14">
-        <v>35</v>
+      <c r="I7" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" ht="18" customHeight="1">
+    <row r="8" spans="1:11" ht="18" customHeight="1">
       <c r="A8" s="20">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="21">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s" s="21">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s" s="27">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s" s="21">
-        <v>13</v>
+      <c r="B8" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="H8" s="24">
         <v>41990</v>
       </c>
-      <c r="I8" t="s" s="21">
-        <v>24</v>
+      <c r="I8" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" ht="19" customHeight="1">
+    <row r="9" spans="1:11" ht="19" customHeight="1">
       <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s" s="14">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s" s="26">
+      <c r="B9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" t="s" s="16">
-        <v>13</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="18">
         <v>41990</v>
       </c>
-      <c r="I9" t="s" s="21">
-        <v>24</v>
+      <c r="I9" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" ht="18" customHeight="1">
+    <row r="10" spans="1:11" ht="18" customHeight="1">
       <c r="A10" s="20">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="21">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s" s="21">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s" s="27">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s" s="21">
-        <v>13</v>
+      <c r="B10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
       <c r="H10" s="24">
         <v>41990</v>
       </c>
-      <c r="I10" t="s" s="21">
-        <v>42</v>
+      <c r="I10" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" ht="19" customHeight="1">
+    <row r="11" spans="1:11" ht="19" customHeight="1">
       <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="21">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s" s="14">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s" s="26">
+      <c r="B11" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="E11" t="s" s="16">
-        <v>13</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18">
         <v>41990</v>
       </c>
-      <c r="I11" t="s" s="21">
-        <v>42</v>
+      <c r="I11" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" ht="19" customHeight="1">
+    <row r="12" spans="1:11" ht="19" customHeight="1">
       <c r="A12" s="20">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="21">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s" s="21">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s" s="22">
+      <c r="B12" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>12</v>
-      </c>
-      <c r="E12" t="s" s="21">
-        <v>13</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
       <c r="H12" s="24">
         <v>41990</v>
       </c>
-      <c r="I12" t="s" s="21">
-        <v>46</v>
+      <c r="I12" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" ht="19" customHeight="1">
+    <row r="13" spans="1:11" ht="19" customHeight="1">
       <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s" s="26">
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" t="s" s="16">
-        <v>13</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="18">
         <v>41990</v>
       </c>
-      <c r="I13" t="s" s="14">
-        <v>46</v>
+      <c r="I13" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" ht="18" customHeight="1">
+    <row r="14" spans="1:11" ht="18" customHeight="1">
       <c r="A14" s="20">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="21">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s" s="21">
-        <v>49</v>
-      </c>
-      <c r="D14" t="s" s="22">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s" s="21">
-        <v>13</v>
+      <c r="B14" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
       <c r="H14" s="24">
         <v>41990</v>
       </c>
-      <c r="I14" t="s" s="14">
-        <v>46</v>
+      <c r="I14" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" ht="18" customHeight="1">
+    <row r="15" spans="1:11" ht="18" customHeight="1">
       <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="28">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s" s="28">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s" s="15">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="16">
-        <v>13</v>
+      <c r="B15" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="18">
         <v>41990</v>
       </c>
-      <c r="I15" t="s" s="14">
-        <v>52</v>
+      <c r="I15" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" ht="18" customHeight="1">
+    <row r="16" spans="1:11" ht="18" customHeight="1">
       <c r="A16" s="20">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="29">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s" s="29">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s" s="29">
-        <v>19</v>
+      <c r="B16" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
-      <c r="I16" t="s" s="21">
-        <v>46</v>
+      <c r="I16" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" ht="18" customHeight="1">
+    <row r="17" spans="1:11" ht="18" customHeight="1">
       <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="28">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s" s="28">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s" s="28">
-        <v>19</v>
+      <c r="B17" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
-      <c r="I17" t="s" s="14">
-        <v>52</v>
+      <c r="I17" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="J17" s="19"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" ht="18" customHeight="1">
+    <row r="18" spans="1:11" ht="18" customHeight="1">
       <c r="A18" s="20">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="29">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s" s="29">
-        <v>57</v>
-      </c>
-      <c r="D18" t="s" s="29">
-        <v>58</v>
+      <c r="B18" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>36</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
-      <c r="I18" t="s" s="21">
-        <v>59</v>
+      <c r="I18" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" ht="18" customHeight="1">
+    <row r="19" spans="1:11" ht="18" customHeight="1">
       <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="29">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s" s="28">
-        <v>60</v>
-      </c>
-      <c r="D19" t="s" s="28">
-        <v>19</v>
+      <c r="B19" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" t="s" s="14">
-        <v>61</v>
+      <c r="I19" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" ht="18" customHeight="1">
+    <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="28">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s" s="28">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s" s="28">
-        <v>58</v>
+      <c r="B20" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" t="s" s="14">
-        <v>64</v>
+      <c r="I20" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" ht="18" customHeight="1">
+    <row r="21" spans="1:11" ht="18" customHeight="1">
       <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="28">
-        <v>65</v>
-      </c>
-      <c r="C21" t="s" s="28">
-        <v>66</v>
-      </c>
-      <c r="D21" t="s" s="28">
-        <v>19</v>
+      <c r="B21" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" t="s" s="14">
-        <v>67</v>
+      <c r="I21" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" ht="18" customHeight="1">
+    <row r="22" spans="1:11" ht="18" customHeight="1">
       <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="29">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s" s="28">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s" s="28">
-        <v>58</v>
+      <c r="B22" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
-      <c r="I22" t="s" s="21">
-        <v>59</v>
+      <c r="I22" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" ht="18" customHeight="1">
+    <row r="23" spans="1:11" ht="18" customHeight="1">
       <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="28">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s" s="28">
-        <v>70</v>
-      </c>
-      <c r="D23" t="s" s="28">
-        <v>58</v>
+      <c r="B23" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
-      <c r="I23" t="s" s="14">
-        <v>71</v>
+      <c r="I23" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="J23" s="19"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" ht="18" customHeight="1">
+    <row r="24" spans="1:11" ht="18" customHeight="1">
       <c r="A24" s="13">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="28">
-        <v>72</v>
-      </c>
-      <c r="C24" t="s" s="28">
-        <v>73</v>
-      </c>
-      <c r="D24" t="s" s="30">
-        <v>58</v>
+      <c r="B24" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -2268,7 +3441,7 @@
       <c r="J24" s="19"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" ht="18" customHeight="1">
+    <row r="25" spans="1:11" ht="18" customHeight="1">
       <c r="A25" s="31"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -2281,7 +3454,7 @@
       <c r="J25" s="19"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" ht="18" customHeight="1">
+    <row r="26" spans="1:11" ht="18" customHeight="1">
       <c r="A26" s="34"/>
       <c r="B26" s="35"/>
       <c r="C26" s="35"/>
@@ -2295,96 +3468,96 @@
       <c r="K26" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="14" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.75" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="38" customWidth="1"/>
-    <col min="2" max="2" width="7.75" style="38" customWidth="1"/>
-    <col min="3" max="3" width="7.75" style="38" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="38" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="38" customWidth="1"/>
-    <col min="6" max="256" width="7.75" style="38" customWidth="1"/>
+    <col min="1" max="256" width="7.75" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1">
+    <row r="1" spans="1:5" ht="18" customHeight="1">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" ht="18" customHeight="1">
+    <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="18" customHeight="1">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" ht="18" customHeight="1">
+    <row r="4" spans="1:5" ht="18" customHeight="1">
       <c r="A4" s="39"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" ht="18" customHeight="1">
+    <row r="5" spans="1:5" ht="18" customHeight="1">
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
     </row>
-    <row r="6" ht="18" customHeight="1">
+    <row r="6" spans="1:5" ht="18" customHeight="1">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" ht="18" customHeight="1">
+    <row r="7" spans="1:5" ht="18" customHeight="1">
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
     </row>
-    <row r="8" ht="18" customHeight="1">
+    <row r="8" spans="1:5" ht="18" customHeight="1">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
     </row>
-    <row r="9" ht="18" customHeight="1">
+    <row r="9" spans="1:5" ht="18" customHeight="1">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
     </row>
-    <row r="10" ht="18" customHeight="1">
+    <row r="10" spans="1:5" ht="18" customHeight="1">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
@@ -2392,94 +3565,95 @@
       <c r="E10" s="39"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="14" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.75" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="40" customWidth="1"/>
-    <col min="2" max="2" width="7.75" style="40" customWidth="1"/>
-    <col min="3" max="3" width="7.75" style="40" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="40" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="40" customWidth="1"/>
-    <col min="6" max="256" width="7.75" style="40" customWidth="1"/>
+    <col min="1" max="256" width="7.75" style="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1">
+    <row r="1" spans="1:5" ht="18" customHeight="1">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" ht="18" customHeight="1">
+    <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="18" customHeight="1">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" ht="18" customHeight="1">
+    <row r="4" spans="1:5" ht="18" customHeight="1">
       <c r="A4" s="39"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" ht="18" customHeight="1">
+    <row r="5" spans="1:5" ht="18" customHeight="1">
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
     </row>
-    <row r="6" ht="18" customHeight="1">
+    <row r="6" spans="1:5" ht="18" customHeight="1">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" ht="18" customHeight="1">
+    <row r="7" spans="1:5" ht="18" customHeight="1">
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
     </row>
-    <row r="8" ht="18" customHeight="1">
+    <row r="8" spans="1:5" ht="18" customHeight="1">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
     </row>
-    <row r="9" ht="18" customHeight="1">
+    <row r="9" spans="1:5" ht="18" customHeight="1">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
     </row>
-    <row r="10" ht="18" customHeight="1">
+    <row r="10" spans="1:5" ht="18" customHeight="1">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
@@ -2487,10 +3661,16 @@
       <c r="E10" s="39"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>